<commit_message>
-have added feature to add firms, cities, regions, end else through seed files.
</commit_message>
<xml_diff>
--- a/Code/Questionnaire.Data/SeedFiles/Cities.xlsx
+++ b/Code/Questionnaire.Data/SeedFiles/Cities.xlsx
@@ -170,7 +170,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,7 +237,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>

</xml_diff>